<commit_message>
Updated Transfer note script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-TransferNote.data.xlsx
+++ b/tests/artifact/data/UI-TransferNote.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6500" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="248">
   <si>
     <t>login.screen</t>
   </si>
@@ -184,7 +184,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>//button[text()=' Open ']</t>
+    <t>(//button[text()=' Open '])[107]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -433,6 +433,12 @@
     <t>//main[@class='mb-5']/section/div/div/div/div[11]/div/table/tbody/tr</t>
   </si>
   <si>
+    <t>tn.table.row.no.xpath</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div/div/div[11]/div/table/tbody/tr/td[2]</t>
+  </si>
+  <si>
     <t>table.dateField.values</t>
   </si>
   <si>
@@ -508,13 +514,13 @@
     <t>tn.dispatch.From.values</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/div/form/div[2]/div[1]/div/div[2]/div[3]/div/div/div/div/input</t>
+    <t>//main[@class='mb-5']/div/form/div[2]/div[1]/div/div[2]/div[3]/div/select</t>
   </si>
   <si>
     <t>tn.dispatch.to.values</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/div/form/div[2]/div[1]/div/div[2]/div[4]/div/div/div/div/input</t>
+    <t>//main[@class='mb-5']/div/form/div[2]/div[1]/div/div[2]/div[4]/div/select</t>
   </si>
   <si>
     <t>tn.issuer.values</t>
@@ -544,7 +550,7 @@
     <t>Enter.date.values</t>
   </si>
   <si>
-    <t>10-11-2023</t>
+    <t>18-12-2023</t>
   </si>
   <si>
     <t>td.dateofsupply.key</t>
@@ -610,12 +616,12 @@
     <t>SupplyDate</t>
   </si>
   <si>
-    <t>13-11-2023</t>
-  </si>
-  <si>
     <t>receiptDate</t>
   </si>
   <si>
+    <t>20-12-2023</t>
+  </si>
+  <si>
     <t>ctn.addItem</t>
   </si>
   <si>
@@ -655,7 +661,7 @@
     <t>ai.CancelorAddbutton</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/div/form/div[3]/div/table/tbody/tr/td[3]/button</t>
+    <t>(//main[@class='mb-5']/div/form/div[3]/div/table/tbody/tr/td[3]/button)[2]</t>
   </si>
   <si>
     <t>backTransferNote.Button</t>
@@ -701,6 +707,78 @@
   </si>
   <si>
     <t>click.Reset.Button</t>
+  </si>
+  <si>
+    <t>transfer.Note.PopUpMessage</t>
+  </si>
+  <si>
+    <t>//div[@class='mr-2'][contains(text(),'Create Transfer Note Successfull!')]</t>
+  </si>
+  <si>
+    <t>click.created.TransferNote</t>
+  </si>
+  <si>
+    <t>//div[@class='d-print-none']/button[1]</t>
+  </si>
+  <si>
+    <t>click.print.button</t>
+  </si>
+  <si>
+    <t>//div[@class='d-print-none']/button[2]</t>
+  </si>
+  <si>
+    <t>xpath.PopUp.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='b-toaster b-toaster-top-right']/div/div/div/header/strong</t>
+  </si>
+  <si>
+    <t>TransferNote.title</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-body px-0']/div/div/h3</t>
+  </si>
+  <si>
+    <t>TransferNoteForm.No</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-body px-0']/div/div[2]/div/div/div[2]/table/tbody/tr[1]/td[2]/span</t>
+  </si>
+  <si>
+    <t>cancel.Transfer.Creation</t>
+  </si>
+  <si>
+    <t>(//div[@class='modal-content'])[4]/footer/button[1]</t>
+  </si>
+  <si>
+    <t>transferNote.Details.No</t>
+  </si>
+  <si>
+    <t>(//div[@class='row'])[3]/div[2]/table/tbody/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>tn.actual.receiptDate</t>
+  </si>
+  <si>
+    <t>(//div[@class='row'])[3]/div[2]/table/tbody/tr[7]/td[2]/div/div/div/input</t>
+  </si>
+  <si>
+    <t>tn.approve.button</t>
+  </si>
+  <si>
+    <t>//div[@class='float-right d-print-none']/button</t>
+  </si>
+  <si>
+    <t>tn.approve.popup.message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'Transfer Note ${tndetailsno} was successfully approved!')]</t>
+  </si>
+  <si>
+    <t>tn.print.Icon</t>
+  </si>
+  <si>
+    <t>//div[@class='card ml-md-2']/div/button[2]</t>
   </si>
 </sst>
 </file>
@@ -1819,10 +1897,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2443,13 +2521,14 @@
       </c>
       <c r="C74" s="8"/>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C75" s="8"/>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
@@ -2624,7 +2703,7 @@
         <v>192</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2744,7 +2823,111 @@
         <v>221</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>210</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2837,40 +3020,26 @@
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(A66))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A66,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A66,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A66,LEN("//"))="//"</formula>
+  <conditionalFormatting sqref="A112">
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A112,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A112,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A112,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A112))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A111))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A111,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A111,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A111,LEN("//"))="//"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B111">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B111))&gt;0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="B112">
     <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(B112))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
@@ -2887,6 +3056,20 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A66:A67">
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A66,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A66,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A66,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
+      <formula>LEN(TRIM(A66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3">
     <cfRule type="expression" dxfId="5" priority="63" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
@@ -2903,7 +3086,7 @@
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E59 B41:B59 B29:B39 B60:E110 C111:E111 B112:E1048576">
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E59 B41:B59 B29:B39 B60:E111 B113:E1048576 C112:E112">
     <cfRule type="expression" dxfId="5" priority="69" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
@@ -2911,7 +3094,7 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A65 A67:A110 A112:A1048576">
+  <conditionalFormatting sqref="A4:A24 A29:A65 A68:A111 A113:A1048576">
     <cfRule type="beginsWith" dxfId="3" priority="65" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Modified the TransferNote script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-TransferNote.data.xlsx
+++ b/tests/artifact/data/UI-TransferNote.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="251">
   <si>
     <t>login.screen</t>
   </si>
@@ -616,16 +616,25 @@
     <t>SupplyDate</t>
   </si>
   <si>
+    <t>27-12-2023</t>
+  </si>
+  <si>
     <t>receiptDate</t>
   </si>
   <si>
-    <t>20-12-2023</t>
+    <t>29-12-2023</t>
   </si>
   <si>
     <t>ctn.addItem</t>
   </si>
   <si>
     <t>//main[@class='mb-5']/div/form/div[3]/div/div/div/span/button/span</t>
+  </si>
+  <si>
+    <t>verify.addedItem</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/div/form/div[3]/div/table/tbody/tr[2]</t>
   </si>
   <si>
     <t>ai.Item</t>
@@ -1897,10 +1906,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B80" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2703,231 +2712,239 @@
         <v>192</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3020,26 +3037,26 @@
       <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A112">
+  <conditionalFormatting sqref="A113">
     <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A112,LEN("//"))="//"</formula>
+      <formula>LEFT(A113,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A112,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A113,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A112,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A113,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A112))&gt;0</formula>
+      <formula>LEN(TRIM(A113))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B112">
+  <conditionalFormatting sqref="B113">
     <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B112))&gt;0</formula>
+      <formula>LEN(TRIM(B113))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
@@ -3086,7 +3103,7 @@
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E59 B41:B59 B29:B39 B60:E111 B113:E1048576 C112:E112">
+  <conditionalFormatting sqref="C1:E3 B4:E19 C20:E21 B22:E24 C25:E59 B41:B59 B29:B39 B60:E112 C113:E113 B114:E1048576">
     <cfRule type="expression" dxfId="5" priority="69" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
@@ -3094,7 +3111,7 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A65 A68:A111 A113:A1048576">
+  <conditionalFormatting sqref="A4:A24 A29:A65 A68:A112 A114:A1048576">
     <cfRule type="beginsWith" dxfId="3" priority="65" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>

</xml_diff>